<commit_message>
Customer module in admin panel
</commit_message>
<xml_diff>
--- a/public/sample-file/Customers-Sample.xlsx
+++ b/public/sample-file/Customers-Sample.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="30" windowWidth="20115" windowHeight="8010"/>
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="clients" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -70,20 +70,20 @@
     <t>hb1@gmail.com</t>
   </si>
   <si>
-    <t>Goa</t>
-  </si>
-  <si>
-    <t>Afghanistan</t>
-  </si>
-  <si>
     <t>Email</t>
+  </si>
+  <si>
+    <t>India</t>
+  </si>
+  <si>
+    <t>Gujarat</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="19" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="19">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -705,7 +705,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -740,7 +739,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -916,21 +914,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M9" sqref="M9"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="4.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="8" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="15.140625" bestFit="1" customWidth="1"/>
@@ -939,7 +937,7 @@
     <col min="12" max="12" width="17.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -968,7 +966,7 @@
         <v>8</v>
       </c>
       <c r="J1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="K1" t="s">
         <v>12</v>
@@ -977,7 +975,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -991,7 +989,7 @@
         <v>19</v>
       </c>
       <c r="E2" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="F2" t="s">
         <v>11</v>
@@ -999,6 +997,9 @@
       <c r="G2">
         <v>380052</v>
       </c>
+      <c r="H2">
+        <v>7418521478</v>
+      </c>
       <c r="I2">
         <v>9979441155</v>
       </c>
@@ -1012,7 +1013,7 @@
         <v>123456</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -1026,7 +1027,7 @@
         <v>19</v>
       </c>
       <c r="E3" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="F3" t="s">
         <v>11</v>

</xml_diff>